<commit_message>
Remade gerbers and CPL file once more after a few minor tweeks for manufacturing.
</commit_message>
<xml_diff>
--- a/CPL_JLCPCB.xlsx
+++ b/CPL_JLCPCB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve"> 62.4500mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -54.6000mm</t>
+    <t xml:space="preserve">  -54.6000mm</t>
   </si>
   <si>
     <t xml:space="preserve"> top</t>
@@ -55,7 +55,7 @@
     <t xml:space="preserve"> 59.9500mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -66.8300mm</t>
+    <t xml:space="preserve">  -66.8300mm</t>
   </si>
   <si>
     <t xml:space="preserve">C3</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve"> 65.4500mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -67.4500mm</t>
+    <t xml:space="preserve">  -67.4500mm</t>
   </si>
   <si>
     <t xml:space="preserve">C4</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve"> 67.7000mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -56.5000mm</t>
+    <t xml:space="preserve">  -56.5000mm</t>
   </si>
   <si>
     <t xml:space="preserve">D1</t>
@@ -82,7 +82,19 @@
     <t xml:space="preserve"> 62.7000mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -60.0000mm</t>
+    <t xml:space="preserve">  -60.0000mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52.3000mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 73.1000mm</t>
   </si>
   <si>
     <t xml:space="preserve">L1</t>
@@ -91,13 +103,13 @@
     <t xml:space="preserve"> 62.4000mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -52.4500mm</t>
+    <t xml:space="preserve">  -52.4500mm</t>
   </si>
   <si>
     <t xml:space="preserve">Q1</t>
   </si>
   <si>
-    <t xml:space="preserve"> -62.1000mm</t>
+    <t xml:space="preserve">  -62.1000mm</t>
   </si>
   <si>
     <t xml:space="preserve">Q2</t>
@@ -106,7 +118,7 @@
     <t xml:space="preserve"> 57.6000mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -52.9500mm</t>
+    <t xml:space="preserve">  -52.9500mm</t>
   </si>
   <si>
     <t xml:space="preserve">Q3</t>
@@ -115,7 +127,7 @@
     <t xml:space="preserve"> 57.2500mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -65.7000mm</t>
+    <t xml:space="preserve">  -65.7000mm</t>
   </si>
   <si>
     <t xml:space="preserve">R1</t>
@@ -124,7 +136,7 @@
     <t xml:space="preserve"> 61.9500mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -64.9000mm</t>
+    <t xml:space="preserve">  -64.9000mm</t>
   </si>
   <si>
     <t xml:space="preserve">R2</t>
@@ -133,7 +145,7 @@
     <t xml:space="preserve"> 69.0000mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -64.8000mm</t>
+    <t xml:space="preserve">  -64.8000mm</t>
   </si>
   <si>
     <t xml:space="preserve">R3</t>
@@ -142,13 +154,13 @@
     <t xml:space="preserve"> 57.1000mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -61.7000mm</t>
+    <t xml:space="preserve">  -61.7000mm</t>
   </si>
   <si>
     <t xml:space="preserve">R4</t>
   </si>
   <si>
-    <t xml:space="preserve"> -63.0000mm</t>
+    <t xml:space="preserve">  -63.0000mm</t>
   </si>
   <si>
     <t xml:space="preserve">R5</t>
@@ -157,7 +169,7 @@
     <t xml:space="preserve"> 57.8000mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -68.4000mm</t>
+    <t xml:space="preserve">  -68.4000mm</t>
   </si>
   <si>
     <t xml:space="preserve">R6</t>
@@ -166,13 +178,13 @@
     <t xml:space="preserve"> 58.6500mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -56.0000mm</t>
+    <t xml:space="preserve">  -56.0000mm</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
-    <t xml:space="preserve"> -67.0500mm</t>
+    <t xml:space="preserve">  -67.0500mm</t>
   </si>
   <si>
     <t xml:space="preserve">U2</t>
@@ -184,7 +196,7 @@
     <t xml:space="preserve"> 68.0000mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> -67.3500mm</t>
+    <t xml:space="preserve">  -67.3500mm</t>
   </si>
 </sst>
 </file>
@@ -321,7 +333,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -446,143 +458,143 @@
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -593,13 +605,13 @@
     </row>
     <row r="16" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -610,44 +622,44 @@
     </row>
     <row r="17" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>54</v>
@@ -659,7 +671,40 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -677,6 +722,27 @@
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>